<commit_message>
Commit 29-12 fine gg
</commit_message>
<xml_diff>
--- a/inputData/codici.xlsx
+++ b/inputData/codici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ircaeu-my.sharepoint.com/personal/matteo_barone_irca_eu/Documents/Desktop/excelMerger/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{D296EC47-D8F9-4FDC-A7CB-58FC652C1A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46A75D00-B975-451C-9C03-757B12754E48}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{D296EC47-D8F9-4FDC-A7CB-58FC652C1A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03673378-DE50-41CB-9943-2F3926A8583C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69F7C347-5BC3-458E-9868-61B6ED7E07FB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10001" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10001" uniqueCount="1153">
   <si>
     <t>Codice parte</t>
   </si>
@@ -3497,9 +3497,6 @@
   </si>
   <si>
     <t>PLACCHETTA CIOCC. FOND 30MM CARREFOUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item                </t>
   </si>
 </sst>
 </file>
@@ -22825,7 +22822,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1153</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -38531,9 +38528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E82504F-663F-4953-9BCF-1EC68A6E8252}">
   <dimension ref="A1:G1077"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>